<commit_message>
Replaced COG_reasoning_transfer.png with a pdf version. Printer-friendly.
</commit_message>
<xml_diff>
--- a/cvpr_submission/experiments/CLEVR_results.xlsx
+++ b/cvpr_submission/experiments/CLEVR_results.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vincentmarois/Desktop/new_cogent_experiments/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vincentmarois/repos/mi-visual-reasoning-pubs/cvpr_submission/experiments/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDC969BB-0C6C-2541-B368-1DE669FC08B8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C90BDB21-F5FB-DB4A-B84D-B0071F1AA13C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="18940" activeTab="1" xr2:uid="{D08C4B1C-069C-E84C-A7EF-726E0385693A}"/>
   </bookViews>
@@ -1339,10 +1339,7 @@
           <c:spPr>
             <a:pattFill prst="ltDnDiag">
               <a:fgClr>
-                <a:schemeClr val="accent5">
-                  <a:lumMod val="60000"/>
-                  <a:lumOff val="40000"/>
-                </a:schemeClr>
+                <a:schemeClr val="accent3"/>
               </a:fgClr>
               <a:bgClr>
                 <a:schemeClr val="accent4"/>
@@ -5118,7 +5115,7 @@
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19"/>

</xml_diff>